<commit_message>
amos editor modification/development 111422
</commit_message>
<xml_diff>
--- a/academycity/data/avi/datasets/excel/world_bank/P_Data_Extract_From_World_Development_Indicators.xlsx
+++ b/academycity/data/avi/datasets/excel/world_bank/P_Data_Extract_From_World_Development_Indicators.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4015" uniqueCount="584">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
@@ -1686,12 +1686,6 @@
   </si>
   <si>
     <t xml:space="preserve">NY.GDP.PCAP.PP.KD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data from database: World Development Indicators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Updated: 09/16/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -1891,10 +1885,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P804"/>
+  <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A787" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M813" activeCellId="0" sqref="M813"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41856,30 +41850,31 @@
         <v>17080.9264709827</v>
       </c>
     </row>
-    <row r="800" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B800" s="1"/>
-      <c r="D800" s="1"/>
-    </row>
-    <row r="801" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B801" s="1"/>
-      <c r="D801" s="1"/>
-    </row>
-    <row r="802" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B802" s="1"/>
-      <c r="D802" s="1"/>
-    </row>
-    <row r="803" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="B803" s="1"/>
-      <c r="D803" s="1"/>
-    </row>
-    <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="0" t="s">
-        <v>556</v>
-      </c>
-    </row>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -41905,46 +41900,46 @@
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="0" width="50.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="0" width="50.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>566</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41952,35 +41947,35 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>573</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41988,35 +41983,35 @@
         <v>552</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>551</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>573</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>2015</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42024,35 +42019,35 @@
         <v>554</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>553</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>584</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>2017</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>